<commit_message>
Se desifra el algoritmo del cuadro mágico
</commit_message>
<xml_diff>
--- a/practica7/magic square.xlsx
+++ b/practica7/magic square.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\digie\source\repos\Lenguajes-de-Interfaz\practica7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACADA5C-7BB2-4482-9545-03F98816913E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2FD35D-CC0E-4924-848E-533471209410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3EBCA96C-DCDF-49B1-A9A5-18DF9D411266}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{3EBCA96C-DCDF-49B1-A9A5-18DF9D411266}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>i+n(n-1)+1</t>
   </si>
@@ -68,6 +68,18 @@
   <si>
     <t>R</t>
   </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>n2-(n-1)</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>incremento</t>
+  </si>
 </sst>
 </file>
 
@@ -88,7 +100,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,6 +122,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -206,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -239,6 +263,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB229345-88BA-407A-ABED-B463736239A9}">
-  <dimension ref="B2:AI45"/>
+  <dimension ref="B1:AK45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" topLeftCell="G19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AA36" sqref="AA36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,22 +592,62 @@
     <col min="2" max="9" width="3.28515625" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
     <col min="11" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="26" width="3.28515625" customWidth="1"/>
+    <col min="12" max="25" width="3.28515625" customWidth="1"/>
+    <col min="26" max="26" width="8.85546875" customWidth="1"/>
     <col min="27" max="27" width="12.28515625" customWidth="1"/>
-    <col min="28" max="37" width="3.28515625" customWidth="1"/>
+    <col min="28" max="28" width="3.28515625" customWidth="1"/>
+    <col min="29" max="29" width="5.7109375" customWidth="1"/>
+    <col min="30" max="37" width="3.28515625" customWidth="1"/>
     <col min="38" max="52" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="O1">
+        <v>3</v>
+      </c>
+      <c r="R1">
+        <v>3</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <f>($R$1+1)/2</f>
+        <v>2</v>
+      </c>
+      <c r="AC2">
+        <v>7</v>
+      </c>
+    </row>
     <row r="3" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" s="4">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="Z3">
+        <v>2</v>
+      </c>
+      <c r="AA3">
+        <v>9</v>
+      </c>
+      <c r="AC3">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:35" x14ac:dyDescent="0.25">
@@ -588,21 +655,39 @@
         <v>3</v>
       </c>
       <c r="C4" s="10">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6">
+        <v>7</v>
+      </c>
+      <c r="Z4">
+        <v>3</v>
+      </c>
+      <c r="AA4">
         <v>4</v>
       </c>
-      <c r="D4" s="6">
-        <v>8</v>
+      <c r="AC4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5" s="9">
         <v>2</v>
+      </c>
+      <c r="Z5">
+        <v>4</v>
+      </c>
+      <c r="AA5">
+        <v>7</v>
+      </c>
+      <c r="AC5">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -611,6 +696,15 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
+      <c r="Z6">
+        <v>5</v>
+      </c>
+      <c r="AA6">
+        <v>5</v>
+      </c>
+      <c r="AC6">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
@@ -628,81 +722,37 @@
       <c r="F7" s="4">
         <v>13</v>
       </c>
-      <c r="K7" s="1">
-        <v>19</v>
-      </c>
-      <c r="L7" s="1">
-        <v>25</v>
-      </c>
-      <c r="M7" s="1">
-        <v>1</v>
-      </c>
-      <c r="N7" s="1">
-        <v>7</v>
-      </c>
-      <c r="O7" s="1">
-        <v>13</v>
-      </c>
-      <c r="P7" s="1">
-        <v>24</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>5</v>
-      </c>
-      <c r="R7" s="1">
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1">
         <v>6</v>
       </c>
-      <c r="S7" s="1">
-        <v>12</v>
-      </c>
-      <c r="T7" s="1">
-        <v>18</v>
-      </c>
-      <c r="U7" s="1">
-        <v>4</v>
-      </c>
-      <c r="V7" s="1">
-        <v>10</v>
-      </c>
-      <c r="W7" s="1">
-        <v>11</v>
-      </c>
-      <c r="X7" s="10">
-        <v>17</v>
-      </c>
-      <c r="Y7" s="1">
-        <v>23</v>
-      </c>
-      <c r="Z7" s="1">
-        <v>9</v>
-      </c>
       <c r="AA7" s="1">
-        <v>15</v>
-      </c>
-      <c r="AB7" s="10">
-        <v>16</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="AB7" s="10"/>
       <c r="AC7" s="10">
-        <v>22</v>
-      </c>
-      <c r="AD7" s="1">
         <v>3</v>
       </c>
-      <c r="AE7" s="1">
-        <v>14</v>
-      </c>
-      <c r="AF7" s="1">
-        <v>20</v>
-      </c>
-      <c r="AG7" s="1">
-        <v>21</v>
-      </c>
-      <c r="AH7" s="1">
-        <v>2</v>
-      </c>
-      <c r="AI7" s="1">
-        <v>8</v>
-      </c>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
     </row>
     <row r="8" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
@@ -720,6 +770,15 @@
       <c r="F8" s="6">
         <v>18</v>
       </c>
+      <c r="Z8" s="10">
+        <v>7</v>
+      </c>
+      <c r="AA8" s="10">
+        <v>6</v>
+      </c>
+      <c r="AC8" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
@@ -737,6 +796,15 @@
       <c r="F9" s="6">
         <v>23</v>
       </c>
+      <c r="Z9" s="10">
+        <v>8</v>
+      </c>
+      <c r="AA9" s="10">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="10">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
@@ -753,6 +821,12 @@
       </c>
       <c r="F10" s="6">
         <v>3</v>
+      </c>
+      <c r="Z10" s="10">
+        <v>9</v>
+      </c>
+      <c r="AA10" s="10">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -878,7 +952,7 @@
       </c>
       <c r="I16" s="11"/>
     </row>
-    <row r="17" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>12</v>
       </c>
@@ -902,7 +976,7 @@
       </c>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
         <v>19</v>
       </c>
@@ -926,7 +1000,7 @@
       </c>
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="7">
         <v>26</v>
       </c>
@@ -950,7 +1024,7 @@
       </c>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:37" x14ac:dyDescent="0.25">
       <c r="T20" t="s">
         <v>10</v>
       </c>
@@ -963,8 +1037,15 @@
       <c r="AA20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AD20" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK20" s="24"/>
+    </row>
+    <row r="21" spans="2:37" x14ac:dyDescent="0.25">
       <c r="Z21">
         <v>1</v>
       </c>
@@ -972,11 +1053,17 @@
         <f>($X$20+1)/2</f>
         <v>3</v>
       </c>
+      <c r="AC21">
+        <v>21</v>
+      </c>
+      <c r="AD21">
+        <v>21</v>
+      </c>
       <c r="AF21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:37" x14ac:dyDescent="0.25">
       <c r="Z22">
         <f>Z21+1</f>
         <v>2</v>
@@ -985,6 +1072,9 @@
         <f>AA21+21</f>
         <v>24</v>
       </c>
+      <c r="AC22">
+        <v>21</v>
+      </c>
       <c r="AD22">
         <v>21</v>
       </c>
@@ -992,19 +1082,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z23">
+    <row r="23" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z23" s="25">
         <f t="shared" ref="Z23:Z45" si="0">Z22+1</f>
         <v>3</v>
       </c>
+      <c r="AA23" s="25">
+        <v>20</v>
+      </c>
+      <c r="AB23" s="25"/>
+      <c r="AC23" s="25">
+        <v>16</v>
+      </c>
       <c r="AD23">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="AF23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>8</v>
       </c>
@@ -1018,14 +1115,20 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="AA24">
+        <v>11</v>
+      </c>
+      <c r="AC24">
+        <v>21</v>
+      </c>
       <c r="AD24">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="AF24">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
         <v>3</v>
       </c>
@@ -1062,8 +1165,15 @@
       <c r="T25">
         <v>2</v>
       </c>
-      <c r="Z25">
-        <f t="shared" si="0"/>
+      <c r="Z25" s="26">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AA25" s="26">
+        <v>7</v>
+      </c>
+      <c r="AB25" s="26"/>
+      <c r="AC25" s="26">
         <v>5</v>
       </c>
       <c r="AD25">
@@ -1073,7 +1183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7">
         <v>4</v>
       </c>
@@ -1087,14 +1197,20 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
+      <c r="AA26">
+        <v>12</v>
+      </c>
+      <c r="AC26">
+        <v>21</v>
+      </c>
       <c r="AD26">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="AF26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1104,6 +1220,12 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
+      <c r="AA27">
+        <v>8</v>
+      </c>
+      <c r="AC27">
+        <v>21</v>
+      </c>
       <c r="AD27">
         <v>21</v>
       </c>
@@ -1111,7 +1233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>17</v>
       </c>
@@ -1131,6 +1253,12 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="AA28">
+        <v>4</v>
+      </c>
+      <c r="AC28">
+        <v>21</v>
+      </c>
       <c r="AD28">
         <v>21</v>
       </c>
@@ -1138,7 +1266,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B29" s="5">
         <v>23</v>
       </c>
@@ -1154,9 +1282,16 @@
       <c r="F29" s="6">
         <v>16</v>
       </c>
-      <c r="Z29">
+      <c r="Z29" s="25">
         <f t="shared" si="0"/>
         <v>9</v>
+      </c>
+      <c r="AA29" s="25">
+        <v>25</v>
+      </c>
+      <c r="AB29" s="25"/>
+      <c r="AC29" s="25">
+        <v>16</v>
       </c>
       <c r="AD29">
         <v>21</v>
@@ -1165,7 +1300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B30" s="5">
         <v>4</v>
       </c>
@@ -1181,10 +1316,17 @@
       <c r="F30" s="6">
         <v>22</v>
       </c>
-      <c r="Z30">
+      <c r="Z30" s="26">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="AA30" s="26">
+        <v>16</v>
+      </c>
+      <c r="AB30" s="26"/>
+      <c r="AC30" s="26">
+        <v>5</v>
+      </c>
       <c r="AD30">
         <v>21</v>
       </c>
@@ -1192,7 +1334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B31" s="5">
         <v>10</v>
       </c>
@@ -1212,8 +1354,14 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="32" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA31">
+        <v>21</v>
+      </c>
+      <c r="AC31">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="7">
         <v>11</v>
       </c>
@@ -1233,8 +1381,14 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA32">
+        <v>17</v>
+      </c>
+      <c r="AC32">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
@@ -1246,8 +1400,14 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AA33">
+        <v>13</v>
+      </c>
+      <c r="AC33">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B34" s="12">
         <v>30</v>
       </c>
@@ -1282,8 +1442,14 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AA34">
+        <v>9</v>
+      </c>
+      <c r="AC34">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B35" s="5">
         <v>38</v>
       </c>
@@ -1317,12 +1483,19 @@
       <c r="M35" s="21"/>
       <c r="N35" s="21"/>
       <c r="O35" s="21"/>
-      <c r="Z35">
+      <c r="Z35" s="26">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AA35" s="26">
+        <v>5</v>
+      </c>
+      <c r="AB35" s="26"/>
+      <c r="AC35" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B36" s="5">
         <v>46</v>
       </c>
@@ -1353,12 +1526,19 @@
       <c r="M36" s="22"/>
       <c r="N36" s="22"/>
       <c r="O36" s="22"/>
-      <c r="Z36">
+      <c r="Z36" s="25">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AA36" s="25">
+        <v>10</v>
+      </c>
+      <c r="AB36" s="25"/>
+      <c r="AC36" s="25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B37" s="5">
         <v>5</v>
       </c>
@@ -1393,8 +1573,14 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="38" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AA37">
+        <v>1</v>
+      </c>
+      <c r="AC37">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B38" s="5">
         <v>13</v>
       </c>
@@ -1420,8 +1606,14 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="39" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AA38">
+        <v>22</v>
+      </c>
+      <c r="AC38">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B39" s="5">
         <v>21</v>
       </c>
@@ -1447,8 +1639,14 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA39">
+        <v>18</v>
+      </c>
+      <c r="AC39">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="7">
         <v>22</v>
       </c>
@@ -1470,39 +1668,74 @@
       <c r="H40" s="16">
         <v>20</v>
       </c>
-      <c r="Z40">
+      <c r="Z40" s="26">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="41" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AA40" s="26">
+        <v>14</v>
+      </c>
+      <c r="AB40" s="26"/>
+      <c r="AC40" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:29" x14ac:dyDescent="0.25">
       <c r="Z41">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="42" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="Z42">
+      <c r="AA41">
+        <v>19</v>
+      </c>
+      <c r="AC41">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="Z42" s="25">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="43" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AA42" s="25">
+        <v>15</v>
+      </c>
+      <c r="AB42" s="25"/>
+      <c r="AC42" s="25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="2:29" x14ac:dyDescent="0.25">
       <c r="Z43">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="44" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AA43">
+        <v>6</v>
+      </c>
+      <c r="AC43">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="2:29" x14ac:dyDescent="0.25">
       <c r="Z44">
         <f>Z43+1</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="45" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AA44">
+        <v>2</v>
+      </c>
+      <c r="AC44">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="2:29" x14ac:dyDescent="0.25">
       <c r="Z45">
         <f t="shared" si="0"/>
         <v>25</v>
+      </c>
+      <c r="AA45">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se terminó de analizar la práctica 7
</commit_message>
<xml_diff>
--- a/practica7/magic square.xlsx
+++ b/practica7/magic square.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\digie\source\repos\Lenguajes-de-Interfaz\practica7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\System asm\Lenguajes-de-Interfaz\practica7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2FD35D-CC0E-4924-848E-533471209410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CEE198-DBF8-4B09-8013-1621D3A57037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{3EBCA96C-DCDF-49B1-A9A5-18DF9D411266}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3EBCA96C-DCDF-49B1-A9A5-18DF9D411266}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>i+n(n-1)+1</t>
   </si>
@@ -79,6 +79,42 @@
   </si>
   <si>
     <t>incremento</t>
+  </si>
+  <si>
+    <t>5+1</t>
+  </si>
+  <si>
+    <t>/6</t>
+  </si>
+  <si>
+    <t>esi</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>2y</t>
+  </si>
+  <si>
+    <t>neg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aumento </t>
   </si>
 </sst>
 </file>
@@ -100,7 +136,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,6 +170,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -230,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -251,6 +293,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -263,9 +308,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -284,7 +332,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -580,13 +628,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB229345-88BA-407A-ABED-B463736239A9}">
-  <dimension ref="B1:AK45"/>
+  <dimension ref="B1:AP45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AA36" sqref="AA36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AL41" sqref="AL41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="9" width="3.28515625" customWidth="1"/>
@@ -601,7 +649,7 @@
     <col min="38" max="52" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:41" x14ac:dyDescent="0.25">
       <c r="O1">
         <v>3</v>
       </c>
@@ -618,7 +666,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Z2">
         <v>1</v>
       </c>
@@ -630,7 +678,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>8</v>
       </c>
@@ -640,17 +688,18 @@
       <c r="D3" s="4">
         <v>6</v>
       </c>
-      <c r="Z3">
+      <c r="Z3" s="28">
         <v>2</v>
       </c>
-      <c r="AA3">
+      <c r="AA3" s="28">
         <v>9</v>
       </c>
-      <c r="AC3">
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="28">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>3</v>
       </c>
@@ -660,17 +709,18 @@
       <c r="D4" s="6">
         <v>7</v>
       </c>
-      <c r="Z4">
-        <v>3</v>
-      </c>
-      <c r="AA4">
+      <c r="Z4" s="22">
+        <v>3</v>
+      </c>
+      <c r="AA4" s="22">
         <v>4</v>
       </c>
-      <c r="AC4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7">
         <v>4</v>
       </c>
@@ -690,7 +740,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -706,7 +756,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>19</v>
       </c>
@@ -722,8 +772,15 @@
       <c r="F7" s="4">
         <v>13</v>
       </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="1">
+        <v>3</v>
+      </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -737,14 +794,14 @@
       <c r="W7" s="1"/>
       <c r="X7" s="10"/>
       <c r="Y7" s="1"/>
-      <c r="Z7" s="1">
+      <c r="Z7" s="27">
         <v>6</v>
       </c>
-      <c r="AA7" s="1">
-        <v>3</v>
-      </c>
-      <c r="AB7" s="10"/>
-      <c r="AC7" s="10">
+      <c r="AA7" s="27">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="27"/>
+      <c r="AC7" s="27">
         <v>3</v>
       </c>
       <c r="AD7" s="1"/>
@@ -754,7 +811,7 @@
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
     </row>
-    <row r="8" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>24</v>
       </c>
@@ -770,17 +827,18 @@
       <c r="F8" s="6">
         <v>18</v>
       </c>
-      <c r="Z8" s="10">
+      <c r="Z8" s="29">
         <v>7</v>
       </c>
-      <c r="AA8" s="10">
+      <c r="AA8" s="29">
         <v>6</v>
       </c>
-      <c r="AC8" s="10">
+      <c r="AB8" s="28"/>
+      <c r="AC8" s="29">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>4</v>
       </c>
@@ -806,7 +864,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>9</v>
       </c>
@@ -829,7 +887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>14</v>
       </c>
@@ -845,8 +903,14 @@
       <c r="F11" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -855,8 +919,26 @@
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
-    </row>
-    <row r="13" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="Z12" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC12">
+        <v>-3</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE12">
+        <v>1</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG12">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B13" s="12">
         <v>33</v>
       </c>
@@ -879,8 +961,11 @@
         <v>25</v>
       </c>
       <c r="I13" s="11"/>
-    </row>
-    <row r="14" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="Z13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>40</v>
       </c>
@@ -903,8 +988,35 @@
         <v>32</v>
       </c>
       <c r="I14" s="11"/>
-    </row>
-    <row r="15" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AG14">
+        <v>-2</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI14">
+        <v>9</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK14">
+        <v>7</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM14">
+        <v>3</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>20</v>
+      </c>
+      <c r="AO14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>47</v>
       </c>
@@ -928,7 +1040,7 @@
       </c>
       <c r="I15" s="11"/>
     </row>
-    <row r="16" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
         <v>5</v>
       </c>
@@ -951,8 +1063,11 @@
         <v>46</v>
       </c>
       <c r="I16" s="11"/>
-    </row>
-    <row r="17" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="AG16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>12</v>
       </c>
@@ -976,7 +1091,7 @@
       </c>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
         <v>19</v>
       </c>
@@ -999,8 +1114,23 @@
         <v>11</v>
       </c>
       <c r="I18" s="11"/>
-    </row>
-    <row r="19" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG18" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI18">
+        <v>1</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="7">
         <v>26</v>
       </c>
@@ -1024,7 +1154,7 @@
       </c>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:39" x14ac:dyDescent="0.25">
       <c r="T20" t="s">
         <v>10</v>
       </c>
@@ -1034,18 +1164,24 @@
       <c r="X20">
         <v>5</v>
       </c>
+      <c r="Z20" t="s">
+        <v>17</v>
+      </c>
       <c r="AA20" t="s">
         <v>9</v>
       </c>
+      <c r="AC20" t="s">
+        <v>26</v>
+      </c>
       <c r="AD20" t="s">
         <v>12</v>
       </c>
       <c r="AF20" t="s">
         <v>11</v>
       </c>
-      <c r="AK20" s="24"/>
-    </row>
-    <row r="21" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="AK20" s="20"/>
+    </row>
+    <row r="21" spans="2:39" x14ac:dyDescent="0.25">
       <c r="Z21">
         <v>1</v>
       </c>
@@ -1063,7 +1199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:39" x14ac:dyDescent="0.25">
       <c r="Z22">
         <f>Z21+1</f>
         <v>2</v>
@@ -1082,16 +1218,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z23" s="25">
+    <row r="23" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z23" s="21">
         <f t="shared" ref="Z23:Z45" si="0">Z22+1</f>
         <v>3</v>
       </c>
-      <c r="AA23" s="25">
+      <c r="AA23" s="21">
         <v>20</v>
       </c>
-      <c r="AB23" s="25"/>
-      <c r="AC23" s="25">
+      <c r="AB23" s="21"/>
+      <c r="AC23" s="21">
         <v>16</v>
       </c>
       <c r="AD23">
@@ -1100,8 +1236,11 @@
       <c r="AF23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="AM23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>8</v>
       </c>
@@ -1128,7 +1267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
         <v>3</v>
       </c>
@@ -1165,15 +1304,15 @@
       <c r="T25">
         <v>2</v>
       </c>
-      <c r="Z25" s="26">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="AA25" s="26">
+      <c r="Z25" s="22">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AA25" s="22">
         <v>7</v>
       </c>
-      <c r="AB25" s="26"/>
-      <c r="AC25" s="26">
+      <c r="AB25" s="22"/>
+      <c r="AC25" s="22">
         <v>5</v>
       </c>
       <c r="AD25">
@@ -1183,7 +1322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7">
         <v>4</v>
       </c>
@@ -1210,7 +1349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1233,7 +1372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>17</v>
       </c>
@@ -1246,7 +1385,7 @@
       <c r="E28" s="3">
         <v>8</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="30">
         <v>15</v>
       </c>
       <c r="Z28">
@@ -1266,7 +1405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B29" s="5">
         <v>23</v>
       </c>
@@ -1279,18 +1418,18 @@
       <c r="E29" s="1">
         <v>14</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="31">
         <v>16</v>
       </c>
-      <c r="Z29" s="25">
+      <c r="Z29" s="21">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AA29" s="25">
+      <c r="AA29" s="21">
         <v>25</v>
       </c>
-      <c r="AB29" s="25"/>
-      <c r="AC29" s="25">
+      <c r="AB29" s="21"/>
+      <c r="AC29" s="21">
         <v>16</v>
       </c>
       <c r="AD29">
@@ -1300,7 +1439,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B30" s="5">
         <v>4</v>
       </c>
@@ -1313,18 +1452,18 @@
       <c r="E30" s="10">
         <v>20</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="31">
         <v>22</v>
       </c>
-      <c r="Z30" s="26">
+      <c r="Z30" s="22">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="AA30" s="26">
+      <c r="AA30" s="22">
         <v>16</v>
       </c>
-      <c r="AB30" s="26"/>
-      <c r="AC30" s="26">
+      <c r="AB30" s="22"/>
+      <c r="AC30" s="22">
         <v>5</v>
       </c>
       <c r="AD30">
@@ -1334,7 +1473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B31" s="5">
         <v>10</v>
       </c>
@@ -1347,7 +1486,7 @@
       <c r="E31" s="10">
         <v>21</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="31">
         <v>3</v>
       </c>
       <c r="Z31">
@@ -1361,7 +1500,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="7">
         <v>11</v>
       </c>
@@ -1374,7 +1513,7 @@
       <c r="E32" s="8">
         <v>2</v>
       </c>
-      <c r="F32" s="9">
+      <c r="F32" s="32">
         <v>9</v>
       </c>
       <c r="Z32">
@@ -1388,7 +1527,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
@@ -1407,7 +1546,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B34" s="12">
         <v>30</v>
       </c>
@@ -1432,12 +1571,12 @@
       <c r="J34" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="L34" s="20" t="s">
+      <c r="L34" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="20"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23"/>
       <c r="Z34">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1448,8 +1587,35 @@
       <c r="AC34">
         <v>21</v>
       </c>
-    </row>
-    <row r="35" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AH34" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI34">
+        <v>4</v>
+      </c>
+      <c r="AJ34" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK34">
+        <v>25</v>
+      </c>
+      <c r="AL34" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM34">
+        <v>21</v>
+      </c>
+      <c r="AN34" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO34">
+        <v>5</v>
+      </c>
+      <c r="AP34">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B35" s="5">
         <v>38</v>
       </c>
@@ -1477,25 +1643,25 @@
       <c r="K35" t="s">
         <v>6</v>
       </c>
-      <c r="L35" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="M35" s="21"/>
-      <c r="N35" s="21"/>
-      <c r="O35" s="21"/>
-      <c r="Z35" s="26">
+      <c r="L35" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="M35" s="24"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="24"/>
+      <c r="Z35" s="22">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="AA35" s="26">
-        <v>5</v>
-      </c>
-      <c r="AB35" s="26"/>
-      <c r="AC35" s="26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AA35" s="22">
+        <v>5</v>
+      </c>
+      <c r="AB35" s="22"/>
+      <c r="AC35" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B36" s="5">
         <v>46</v>
       </c>
@@ -1520,25 +1686,25 @@
       <c r="J36" t="s">
         <v>2</v>
       </c>
-      <c r="L36" s="22" t="s">
+      <c r="L36" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="22"/>
-      <c r="Z36" s="25">
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="25"/>
+      <c r="Z36" s="21">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="AA36" s="25">
+      <c r="AA36" s="21">
         <v>10</v>
       </c>
-      <c r="AB36" s="25"/>
-      <c r="AC36" s="25">
+      <c r="AB36" s="21"/>
+      <c r="AC36" s="21">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B37" s="5">
         <v>5</v>
       </c>
@@ -1563,12 +1729,12 @@
       <c r="J37" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="L37" s="23" t="s">
+      <c r="L37" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M37" s="23"/>
-      <c r="N37" s="23"/>
-      <c r="O37" s="23"/>
+      <c r="M37" s="26"/>
+      <c r="N37" s="26"/>
+      <c r="O37" s="26"/>
       <c r="Z37">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1579,8 +1745,11 @@
       <c r="AC37">
         <v>21</v>
       </c>
-    </row>
-    <row r="38" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AK37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B38" s="5">
         <v>13</v>
       </c>
@@ -1613,7 +1782,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B39" s="5">
         <v>21</v>
       </c>
@@ -1646,7 +1815,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="7">
         <v>22</v>
       </c>
@@ -1668,19 +1837,19 @@
       <c r="H40" s="16">
         <v>20</v>
       </c>
-      <c r="Z40" s="26">
+      <c r="Z40" s="22">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="AA40" s="26">
+      <c r="AA40" s="22">
         <v>14</v>
       </c>
-      <c r="AB40" s="26"/>
-      <c r="AC40" s="26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AB40" s="22"/>
+      <c r="AC40" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:42" x14ac:dyDescent="0.25">
       <c r="Z41">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1692,20 +1861,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="Z42" s="25">
+    <row r="42" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="Z42" s="21">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="AA42" s="25">
+      <c r="AA42" s="21">
         <v>15</v>
       </c>
-      <c r="AB42" s="25"/>
-      <c r="AC42" s="25">
+      <c r="AB42" s="21"/>
+      <c r="AC42" s="21">
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:42" x14ac:dyDescent="0.25">
       <c r="Z43">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1717,7 +1886,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:42" x14ac:dyDescent="0.25">
       <c r="Z44">
         <f>Z43+1</f>
         <v>24</v>
@@ -1729,7 +1898,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:42" x14ac:dyDescent="0.25">
       <c r="Z45">
         <f t="shared" si="0"/>
         <v>25</v>

</xml_diff>

<commit_message>
Trabajando en práctica 7
El programa lee el numero y ya empieza a colocar los valores en el nuevo acomodo, falta regresar al comienzo del arreglo cuando el incremento pueda ser mayor que el tamaño del cuadrado
</commit_message>
<xml_diff>
--- a/practica7/magic square.xlsx
+++ b/practica7/magic square.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\System asm\Lenguajes-de-Interfaz\practica7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\digie\source\repos\Lenguajes-de-Interfaz\practica7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CEE198-DBF8-4B09-8013-1621D3A57037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71423FFB-BF58-441D-9B6A-83198FB118AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3EBCA96C-DCDF-49B1-A9A5-18DF9D411266}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{3EBCA96C-DCDF-49B1-A9A5-18DF9D411266}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -296,6 +296,12 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -308,12 +314,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -332,7 +332,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -630,11 +630,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB229345-88BA-407A-ABED-B463736239A9}">
   <dimension ref="B1:AP45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AL41" sqref="AL41"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="9" width="3.28515625" customWidth="1"/>
@@ -688,14 +688,14 @@
       <c r="D3" s="4">
         <v>6</v>
       </c>
-      <c r="Z3" s="28">
+      <c r="Z3" s="24">
         <v>2</v>
       </c>
-      <c r="AA3" s="28">
+      <c r="AA3" s="24">
         <v>9</v>
       </c>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="28">
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="24">
         <v>4</v>
       </c>
     </row>
@@ -794,14 +794,14 @@
       <c r="W7" s="1"/>
       <c r="X7" s="10"/>
       <c r="Y7" s="1"/>
-      <c r="Z7" s="27">
+      <c r="Z7" s="23">
         <v>6</v>
       </c>
-      <c r="AA7" s="27">
-        <v>3</v>
-      </c>
-      <c r="AB7" s="27"/>
-      <c r="AC7" s="27">
+      <c r="AA7" s="23">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="23"/>
+      <c r="AC7" s="23">
         <v>3</v>
       </c>
       <c r="AD7" s="1"/>
@@ -827,14 +827,14 @@
       <c r="F8" s="6">
         <v>18</v>
       </c>
-      <c r="Z8" s="29">
+      <c r="Z8" s="25">
         <v>7</v>
       </c>
-      <c r="AA8" s="29">
+      <c r="AA8" s="25">
         <v>6</v>
       </c>
-      <c r="AB8" s="28"/>
-      <c r="AC8" s="29">
+      <c r="AB8" s="24"/>
+      <c r="AC8" s="25">
         <v>4</v>
       </c>
     </row>
@@ -1385,7 +1385,7 @@
       <c r="E28" s="3">
         <v>8</v>
       </c>
-      <c r="F28" s="30">
+      <c r="F28" s="26">
         <v>15</v>
       </c>
       <c r="Z28">
@@ -1418,7 +1418,7 @@
       <c r="E29" s="1">
         <v>14</v>
       </c>
-      <c r="F29" s="31">
+      <c r="F29" s="27">
         <v>16</v>
       </c>
       <c r="Z29" s="21">
@@ -1452,7 +1452,7 @@
       <c r="E30" s="10">
         <v>20</v>
       </c>
-      <c r="F30" s="31">
+      <c r="F30" s="27">
         <v>22</v>
       </c>
       <c r="Z30" s="22">
@@ -1486,7 +1486,7 @@
       <c r="E31" s="10">
         <v>21</v>
       </c>
-      <c r="F31" s="31">
+      <c r="F31" s="27">
         <v>3</v>
       </c>
       <c r="Z31">
@@ -1513,7 +1513,7 @@
       <c r="E32" s="8">
         <v>2</v>
       </c>
-      <c r="F32" s="32">
+      <c r="F32" s="28">
         <v>9</v>
       </c>
       <c r="Z32">
@@ -1571,12 +1571,12 @@
       <c r="J34" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="L34" s="23" t="s">
+      <c r="L34" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="M34" s="23"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="23"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="29"/>
+      <c r="O34" s="29"/>
       <c r="Z34">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1643,12 +1643,12 @@
       <c r="K35" t="s">
         <v>6</v>
       </c>
-      <c r="L35" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="M35" s="24"/>
-      <c r="N35" s="24"/>
-      <c r="O35" s="24"/>
+      <c r="L35" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="M35" s="30"/>
+      <c r="N35" s="30"/>
+      <c r="O35" s="30"/>
       <c r="Z35" s="22">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1686,12 +1686,12 @@
       <c r="J36" t="s">
         <v>2</v>
       </c>
-      <c r="L36" s="25" t="s">
+      <c r="L36" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="25"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="31"/>
+      <c r="O36" s="31"/>
       <c r="Z36" s="21">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1729,12 +1729,12 @@
       <c r="J37" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="L37" s="26" t="s">
+      <c r="L37" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="M37" s="26"/>
-      <c r="N37" s="26"/>
-      <c r="O37" s="26"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="32"/>
+      <c r="O37" s="32"/>
       <c r="Z37">
         <f t="shared" si="0"/>
         <v>17</v>

</xml_diff>

<commit_message>
SE RESOLVIÓ EL ALGORITMO DEL CUADRO MÁGICO
La solución es guardada en un arreglo, falta imprimir los valores en un archivo
</commit_message>
<xml_diff>
--- a/practica7/magic square.xlsx
+++ b/practica7/magic square.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\digie\source\repos\Lenguajes-de-Interfaz\practica7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71423FFB-BF58-441D-9B6A-83198FB118AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8059BDD-736D-45BD-B71B-88E7A22AA967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{3EBCA96C-DCDF-49B1-A9A5-18DF9D411266}"/>
   </bookViews>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB229345-88BA-407A-ABED-B463736239A9}">
   <dimension ref="B1:AP45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,19 +758,19 @@
     </row>
     <row r="7" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="3">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="3">
         <v>1</v>
       </c>
       <c r="E7" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F7" s="4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
         <v>15</v>
@@ -813,19 +813,19 @@
     </row>
     <row r="8" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1">
         <v>5</v>
       </c>
       <c r="D8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F8" s="6">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Z8" s="25">
         <v>7</v>
@@ -843,16 +843,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E9" s="10">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F9" s="6">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Z9" s="10">
         <v>8</v>
@@ -866,16 +866,16 @@
     </row>
     <row r="10" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D10" s="10">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E10" s="10">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="6">
         <v>3</v>
@@ -889,19 +889,19 @@
     </row>
     <row r="11" spans="2:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C11" s="8">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="8">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E11" s="8">
         <v>2</v>
       </c>
       <c r="F11" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AC11" t="s">
         <v>21</v>

</xml_diff>